<commit_message>
Some minor UI tweaks
</commit_message>
<xml_diff>
--- a/IndustrialParamedics/Field_Order_Template.xlsx
+++ b/IndustrialParamedics/Field_Order_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="6700" windowWidth="27640" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="8280" windowWidth="27640" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Job Number:</t>
   </si>
@@ -280,6 +280,9 @@
   <si>
     <t>%OrderForm.orderLines.reasonCode</t>
   </si>
+  <si>
+    <t>%OrderForm.orderLines.item</t>
+  </si>
 </sst>
 </file>
 
@@ -637,6 +640,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -644,29 +669,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -991,7 +994,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B16" sqref="B16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,10 +1013,10 @@
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="51"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1025,10 +1028,10 @@
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="51"/>
+      <c r="I2" s="48"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1131,19 +1134,19 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1161,19 +1164,19 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="52" t="s">
+      <c r="G13" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -1215,13 +1218,13 @@
       <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="54"/>
+      <c r="B16" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="20" t="s">
         <v>30</v>
       </c>
@@ -1234,187 +1237,187 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="54"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="54"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="54"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="54"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="46"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="54"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="54"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="46"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="54"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="46"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="54"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="46"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="54"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="46"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="54"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="46"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="54"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="46"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="54"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="46"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="54"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="54"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="54"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20" t="s">
         <v>2</v>
@@ -1423,33 +1426,33 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="54"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="46"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="54"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="46"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
       <c r="I35" s="20"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
@@ -1494,67 +1497,67 @@
         <v>18</v>
       </c>
       <c r="B40" s="24"/>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="25"/>
@@ -1570,19 +1573,19 @@
       <c r="I45" s="28"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="49" t="s">
+      <c r="A46" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
       <c r="E46" s="29"/>
       <c r="F46" s="29"/>
-      <c r="G46" s="44" t="s">
+      <c r="G46" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H46" s="45"/>
-      <c r="I46" s="46"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="52"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
@@ -1604,19 +1607,19 @@
         <v>22</v>
       </c>
       <c r="B48" s="35"/>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
       <c r="F48" s="29"/>
       <c r="G48" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="I48" s="46"/>
+      <c r="I48" s="52"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="37"/>
@@ -1635,11 +1638,11 @@
       <c r="A50" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="B50" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="29"/>
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
@@ -1659,33 +1662,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="G13:I13"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="B50:D50"/>
@@ -1696,6 +1672,33 @@
     <mergeCell ref="A44:I44"/>
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="G46:I46"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" display="mailto:billings@ipsems.com"/>

</xml_diff>